<commit_message>
Add more pseudocode, including backpropagation.
</commit_message>
<xml_diff>
--- a/Planning/Planning.xlsx
+++ b/Planning/Planning.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647AC5A8-366B-4679-9E05-719162C9BBB8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -137,15 +138,6 @@
     <t>GamePhase</t>
   </si>
   <si>
-    <t>PLACEMENT
-MOVEMENT</t>
-  </si>
-  <si>
-    <t>Square[][] squares
-int turnNumber
-GamePhase phase</t>
-  </si>
-  <si>
     <t>MCTSAgent.train(MCTSAgent.treeRoot, 60)</t>
   </si>
   <si>
@@ -167,11 +159,22 @@
     <t>Board getNextBoard(Board, Delta)
 Node getNextNode(Node)</t>
   </si>
+  <si>
+    <t>PLACEMENT
+MOVEMENT
+FINISHED</t>
+  </si>
+  <si>
+    <t>Square[][] squares
+int turnNumber
+GamePhase phase
+String winner (B or W)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -487,11 +490,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -588,6 +591,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -623,6 +643,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -798,11 +835,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="42.42578125" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -847,10 +884,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>34</v>
@@ -861,11 +898,11 @@
       <c r="F2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="27" t="s">
-        <v>39</v>
+      <c r="H2" s="26" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="31.5" x14ac:dyDescent="0.35">
@@ -879,7 +916,7 @@
         <v>27</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -889,7 +926,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="H5" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -899,7 +936,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -941,7 +978,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -986,7 +1023,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -1003,7 +1040,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AJ25"/>
   <sheetViews>
     <sheetView zoomScale="99" zoomScaleNormal="235" workbookViewId="0">
@@ -1489,134 +1526,134 @@
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="G10" s="26" t="s">
+      <c r="G10" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="26"/>
-      <c r="Q10" s="26"/>
-      <c r="R10" s="26"/>
-      <c r="S10" s="26"/>
-      <c r="T10" s="26"/>
-      <c r="U10" s="26"/>
-      <c r="V10" s="26"/>
-      <c r="W10" s="26"/>
-      <c r="X10" s="26"/>
-      <c r="Y10" s="26"/>
-      <c r="Z10" s="26"/>
-      <c r="AA10" s="26"/>
-      <c r="AB10" s="26"/>
-      <c r="AC10" s="26"/>
-      <c r="AD10" s="26"/>
-      <c r="AE10" s="26"/>
-      <c r="AF10" s="26"/>
-      <c r="AG10" s="26"/>
-      <c r="AH10" s="26"/>
-      <c r="AI10" s="26"/>
-      <c r="AJ10" s="26"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="27"/>
+      <c r="R10" s="27"/>
+      <c r="S10" s="27"/>
+      <c r="T10" s="27"/>
+      <c r="U10" s="27"/>
+      <c r="V10" s="27"/>
+      <c r="W10" s="27"/>
+      <c r="X10" s="27"/>
+      <c r="Y10" s="27"/>
+      <c r="Z10" s="27"/>
+      <c r="AA10" s="27"/>
+      <c r="AB10" s="27"/>
+      <c r="AC10" s="27"/>
+      <c r="AD10" s="27"/>
+      <c r="AE10" s="27"/>
+      <c r="AF10" s="27"/>
+      <c r="AG10" s="27"/>
+      <c r="AH10" s="27"/>
+      <c r="AI10" s="27"/>
+      <c r="AJ10" s="27"/>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="26"/>
-      <c r="R11" s="26"/>
-      <c r="S11" s="26"/>
-      <c r="T11" s="26"/>
-      <c r="U11" s="26"/>
-      <c r="V11" s="26"/>
-      <c r="W11" s="26"/>
-      <c r="X11" s="26"/>
-      <c r="Y11" s="26"/>
-      <c r="Z11" s="26"/>
-      <c r="AA11" s="26"/>
-      <c r="AB11" s="26"/>
-      <c r="AC11" s="26"/>
-      <c r="AD11" s="26"/>
-      <c r="AE11" s="26"/>
-      <c r="AF11" s="26"/>
-      <c r="AG11" s="26"/>
-      <c r="AH11" s="26"/>
-      <c r="AI11" s="26"/>
-      <c r="AJ11" s="26"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="27"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="27"/>
+      <c r="S11" s="27"/>
+      <c r="T11" s="27"/>
+      <c r="U11" s="27"/>
+      <c r="V11" s="27"/>
+      <c r="W11" s="27"/>
+      <c r="X11" s="27"/>
+      <c r="Y11" s="27"/>
+      <c r="Z11" s="27"/>
+      <c r="AA11" s="27"/>
+      <c r="AB11" s="27"/>
+      <c r="AC11" s="27"/>
+      <c r="AD11" s="27"/>
+      <c r="AE11" s="27"/>
+      <c r="AF11" s="27"/>
+      <c r="AG11" s="27"/>
+      <c r="AH11" s="27"/>
+      <c r="AI11" s="27"/>
+      <c r="AJ11" s="27"/>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="26"/>
-      <c r="R12" s="26"/>
-      <c r="S12" s="26"/>
-      <c r="T12" s="26"/>
-      <c r="U12" s="26"/>
-      <c r="V12" s="26"/>
-      <c r="W12" s="26"/>
-      <c r="X12" s="26"/>
-      <c r="Y12" s="26"/>
-      <c r="Z12" s="26"/>
-      <c r="AA12" s="26"/>
-      <c r="AB12" s="26"/>
-      <c r="AC12" s="26"/>
-      <c r="AD12" s="26"/>
-      <c r="AE12" s="26"/>
-      <c r="AF12" s="26"/>
-      <c r="AG12" s="26"/>
-      <c r="AH12" s="26"/>
-      <c r="AI12" s="26"/>
-      <c r="AJ12" s="26"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
+      <c r="Q12" s="27"/>
+      <c r="R12" s="27"/>
+      <c r="S12" s="27"/>
+      <c r="T12" s="27"/>
+      <c r="U12" s="27"/>
+      <c r="V12" s="27"/>
+      <c r="W12" s="27"/>
+      <c r="X12" s="27"/>
+      <c r="Y12" s="27"/>
+      <c r="Z12" s="27"/>
+      <c r="AA12" s="27"/>
+      <c r="AB12" s="27"/>
+      <c r="AC12" s="27"/>
+      <c r="AD12" s="27"/>
+      <c r="AE12" s="27"/>
+      <c r="AF12" s="27"/>
+      <c r="AG12" s="27"/>
+      <c r="AH12" s="27"/>
+      <c r="AI12" s="27"/>
+      <c r="AJ12" s="27"/>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="26"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="26"/>
-      <c r="S13" s="26"/>
-      <c r="T13" s="26"/>
-      <c r="U13" s="26"/>
-      <c r="V13" s="26"/>
-      <c r="W13" s="26"/>
-      <c r="X13" s="26"/>
-      <c r="Y13" s="26"/>
-      <c r="Z13" s="26"/>
-      <c r="AA13" s="26"/>
-      <c r="AB13" s="26"/>
-      <c r="AC13" s="26"/>
-      <c r="AD13" s="26"/>
-      <c r="AE13" s="26"/>
-      <c r="AF13" s="26"/>
-      <c r="AG13" s="26"/>
-      <c r="AH13" s="26"/>
-      <c r="AI13" s="26"/>
-      <c r="AJ13" s="26"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
+      <c r="Q13" s="27"/>
+      <c r="R13" s="27"/>
+      <c r="S13" s="27"/>
+      <c r="T13" s="27"/>
+      <c r="U13" s="27"/>
+      <c r="V13" s="27"/>
+      <c r="W13" s="27"/>
+      <c r="X13" s="27"/>
+      <c r="Y13" s="27"/>
+      <c r="Z13" s="27"/>
+      <c r="AA13" s="27"/>
+      <c r="AB13" s="27"/>
+      <c r="AC13" s="27"/>
+      <c r="AD13" s="27"/>
+      <c r="AE13" s="27"/>
+      <c r="AF13" s="27"/>
+      <c r="AG13" s="27"/>
+      <c r="AH13" s="27"/>
+      <c r="AI13" s="27"/>
+      <c r="AJ13" s="27"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>

</xml_diff>

<commit_message>
Make changes/additions to plans
</commit_message>
<xml_diff>
--- a/Planning/Planning.xlsx
+++ b/Planning/Planning.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647AC5A8-366B-4679-9E05-719162C9BBB8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E85889-5A99-44B8-8FB5-EED8BD0B97B4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -101,11 +101,6 @@
     <t>Consider starting with a board. Every following board has a delta associated with it. This will make it easy to keep track of changes</t>
   </si>
   <si>
-    <t xml:space="preserve">
-String color (B or W)
-String representation (e.g. @ or O)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -136,16 +131,6 @@
   </si>
   <si>
     <t>GamePhase</t>
-  </si>
-  <si>
-    <t>MCTSAgent.train(MCTSAgent.treeRoot, 60)</t>
-  </si>
-  <si>
-    <t>Node treeRoot
-void train(Node root, int seconds)
-void select(Node startNode)
-void expand(Node node)
-void simulate(Node node)</t>
   </si>
   <si>
     <t>Node parent
@@ -156,19 +141,42 @@
 Delta delta</t>
   </si>
   <si>
-    <t>Board getNextBoard(Board, Delta)
-Node getNextNode(Node)</t>
-  </si>
-  <si>
     <t>PLACEMENT
 MOVEMENT
 FINISHED</t>
   </si>
   <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>WHITE
+BLACK
+.getRepresentation() (@ or O)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Player owner</t>
+  </si>
+  <si>
     <t>Square[][] squares
-int turnNumber
+int roundNumber
 GamePhase phase
-String winner (B or W)</t>
+Player winner</t>
+  </si>
+  <si>
+    <t>Utils</t>
+  </si>
+  <si>
+    <t>Board getNextBoard(Board, Delta)</t>
+  </si>
+  <si>
+    <t>Node treeRoot</t>
+  </si>
+  <si>
+    <t>void train(Node root, int seconds)
+void select(Node node, int Ni)
+void simulate(Node node)
+void backPropogate(Node node, Player winner)</t>
   </si>
 </sst>
 </file>
@@ -836,10 +844,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="42.42578125" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -850,10 +858,11 @@
     <col min="4" max="4" width="23.28515625" customWidth="1"/>
     <col min="5" max="5" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" width="45.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -873,61 +882,65 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="91.5" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="91.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G2" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H2" s="26" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="31.5" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="61.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+      <c r="I3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="H5" s="4" t="s">
-        <v>36</v>
-      </c>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -982,7 +995,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.5703125" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -996,10 +1009,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1012,6 +1028,9 @@
       <c r="C2" t="s">
         <v>13</v>
       </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
@@ -1023,7 +1042,10 @@
         <v>14</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add additional functionalities and documentation
</commit_message>
<xml_diff>
--- a/Planning/Planning.xlsx
+++ b/Planning/Planning.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F570E9-9BE6-48E6-B718-D88186816C84}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6BF4DD-C545-4DD9-B4FF-14E4D3FB7216}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -1063,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AJ25"/>
+  <dimension ref="A1:AR25"/>
   <sheetViews>
     <sheetView zoomScale="99" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="AG3" sqref="AG3"/>
+      <selection activeCell="AN3" sqref="AN3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,7 +1074,7 @@
     <col min="1" max="16384" width="2.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -1135,8 +1135,20 @@
       <c r="AI1" s="9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL1" s="7"/>
+      <c r="AM1" s="8"/>
+      <c r="AN1" s="7"/>
+      <c r="AO1" s="8"/>
+      <c r="AP1" s="7"/>
+      <c r="AQ1" s="8"/>
+      <c r="AR1" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
       <c r="C2" s="12"/>
@@ -1190,8 +1202,16 @@
       <c r="AG2" s="11"/>
       <c r="AH2" s="12"/>
       <c r="AI2" s="13"/>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK2" s="10"/>
+      <c r="AL2" s="11"/>
+      <c r="AM2" s="12"/>
+      <c r="AN2" s="11"/>
+      <c r="AO2" s="12"/>
+      <c r="AP2" s="11"/>
+      <c r="AQ2" s="12"/>
+      <c r="AR2" s="13"/>
+    </row>
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>17</v>
       </c>
@@ -1249,8 +1269,22 @@
         <v>18</v>
       </c>
       <c r="AI3" s="15"/>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK3" s="14"/>
+      <c r="AL3" s="12"/>
+      <c r="AM3" s="11"/>
+      <c r="AN3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="AO3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="AP3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="AQ3" s="11"/>
+      <c r="AR3" s="15"/>
+    </row>
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="11"/>
       <c r="C4" s="12"/>
@@ -1310,8 +1344,16 @@
       </c>
       <c r="AH4" s="12"/>
       <c r="AI4" s="13"/>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK4" s="10"/>
+      <c r="AL4" s="11"/>
+      <c r="AM4" s="12"/>
+      <c r="AN4" s="11"/>
+      <c r="AO4" s="12"/>
+      <c r="AP4" s="11"/>
+      <c r="AQ4" s="12"/>
+      <c r="AR4" s="13"/>
+    </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>17</v>
       </c>
@@ -1377,8 +1419,16 @@
       <c r="AG5" s="12"/>
       <c r="AH5" s="11"/>
       <c r="AI5" s="15"/>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK5" s="14"/>
+      <c r="AL5" s="12"/>
+      <c r="AM5" s="11"/>
+      <c r="AN5" s="12"/>
+      <c r="AO5" s="11"/>
+      <c r="AP5" s="12"/>
+      <c r="AQ5" s="11"/>
+      <c r="AR5" s="15"/>
+    </row>
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="11" t="s">
         <v>18</v>
@@ -1444,8 +1494,16 @@
       <c r="AG6" s="11"/>
       <c r="AH6" s="12"/>
       <c r="AI6" s="13"/>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK6" s="10"/>
+      <c r="AL6" s="11"/>
+      <c r="AM6" s="12"/>
+      <c r="AN6" s="11"/>
+      <c r="AO6" s="12"/>
+      <c r="AP6" s="11"/>
+      <c r="AQ6" s="12"/>
+      <c r="AR6" s="13"/>
+    </row>
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="12" t="s">
         <v>18</v>
@@ -1496,8 +1554,16 @@
       <c r="AG7" s="12"/>
       <c r="AH7" s="11"/>
       <c r="AI7" s="15"/>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK7" s="14"/>
+      <c r="AL7" s="12"/>
+      <c r="AM7" s="11"/>
+      <c r="AN7" s="12"/>
+      <c r="AO7" s="11"/>
+      <c r="AP7" s="12"/>
+      <c r="AQ7" s="11"/>
+      <c r="AR7" s="15"/>
+    </row>
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>16</v>
       </c>
@@ -1546,8 +1612,20 @@
       <c r="AI8" s="19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL8" s="17"/>
+      <c r="AM8" s="18"/>
+      <c r="AN8" s="17"/>
+      <c r="AO8" s="18"/>
+      <c r="AP8" s="17"/>
+      <c r="AQ8" s="18"/>
+      <c r="AR8" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="G10" s="27" t="s">
         <v>25</v>
       </c>
@@ -1581,7 +1659,7 @@
       <c r="AI10" s="27"/>
       <c r="AJ10" s="27"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="G11" s="27"/>
       <c r="H11" s="27"/>
       <c r="I11" s="27"/>
@@ -1613,7 +1691,7 @@
       <c r="AI11" s="27"/>
       <c r="AJ11" s="27"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="G12" s="27"/>
       <c r="H12" s="27"/>
       <c r="I12" s="27"/>
@@ -1645,7 +1723,7 @@
       <c r="AI12" s="27"/>
       <c r="AJ12" s="27"/>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="G13" s="27"/>
       <c r="H13" s="27"/>
       <c r="I13" s="27"/>
@@ -1678,14 +1756,18 @@
       <c r="AJ13" s="27"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
+      <c r="A18" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
       <c r="D18" s="7"/>
       <c r="E18" s="8"/>
       <c r="F18" s="7"/>
       <c r="G18" s="8"/>
-      <c r="H18" s="9"/>
+      <c r="H18" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
@@ -1748,14 +1830,18 @@
       <c r="H24" s="15"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
+      <c r="A25" s="16" t="s">
+        <v>16</v>
+      </c>
       <c r="B25" s="17"/>
       <c r="C25" s="18"/>
       <c r="D25" s="17"/>
       <c r="E25" s="18"/>
       <c r="F25" s="17"/>
       <c r="G25" s="18"/>
-      <c r="H25" s="19"/>
+      <c r="H25" s="19" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Fix complicated issue with death zones
See "Bug 2" text under Part B Notes.txt for more details. Might require
more testing to make sure that it's fixed.
</commit_message>
<xml_diff>
--- a/Planning/Planning.xlsx
+++ b/Planning/Planning.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4973C0-E74E-47D0-92D7-D702EE96ED50}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584C5119-0880-4482-893D-75C67E646FA8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -183,7 +183,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,6 +230,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -425,7 +432,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -503,6 +510,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1063,10 +1073,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:BB26"/>
+  <dimension ref="A1:BA26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AS1" zoomScale="385" zoomScaleNormal="385" workbookViewId="0">
-      <selection activeCell="BB3" sqref="BB3"/>
+      <selection activeCell="AW2" sqref="AW2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,7 +1084,7 @@
     <col min="1" max="16384" width="2.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
       <c r="AT1" s="5">
         <v>0</v>
       </c>
@@ -1100,7 +1110,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
@@ -1179,26 +1189,17 @@
       <c r="AT2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="AU2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="AV2" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="AU2" s="7"/>
+      <c r="AV2" s="8"/>
       <c r="AW2" s="7"/>
       <c r="AX2" s="8"/>
-      <c r="AY2" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="AY2" s="7"/>
       <c r="AZ2" s="8"/>
       <c r="BA2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="BB2" s="5">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
       <c r="C3" s="12"/>
@@ -1264,21 +1265,17 @@
         <v>1</v>
       </c>
       <c r="AT3" s="10"/>
-      <c r="AU3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="AV3" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="AU3" s="11"/>
+      <c r="AV3" s="12"/>
       <c r="AW3" s="11"/>
       <c r="AX3" s="12"/>
       <c r="AY3" s="11"/>
-      <c r="AZ3" s="12"/>
-      <c r="BA3" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="AZ3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="BA3" s="13"/>
+    </row>
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>17</v>
       </c>
@@ -1353,22 +1350,18 @@
       <c r="AS4" s="5">
         <v>2</v>
       </c>
-      <c r="AT4" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="AU4" s="12" t="s">
-        <v>18</v>
-      </c>
+      <c r="AT4" s="14"/>
+      <c r="AU4" s="12"/>
       <c r="AV4" s="11"/>
-      <c r="AW4" s="12" t="s">
-        <v>18</v>
-      </c>
+      <c r="AW4" s="12"/>
       <c r="AX4" s="11"/>
       <c r="AY4" s="12"/>
-      <c r="AZ4" s="11"/>
+      <c r="AZ4" s="11" t="s">
+        <v>18</v>
+      </c>
       <c r="BA4" s="15"/>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
@@ -1441,20 +1434,18 @@
       </c>
       <c r="AT5" s="10"/>
       <c r="AU5" s="11"/>
-      <c r="AV5" s="12" t="s">
-        <v>18</v>
-      </c>
+      <c r="AV5" s="12"/>
       <c r="AW5" s="11"/>
-      <c r="AX5" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="AY5" s="11"/>
-      <c r="AZ5" s="12"/>
-      <c r="BA5" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="AX5" s="12"/>
+      <c r="AY5" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="AZ5" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="BA5" s="13"/>
+    </row>
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>17</v>
       </c>
@@ -1531,22 +1522,16 @@
       <c r="AS6" s="5">
         <v>4</v>
       </c>
-      <c r="AT6" s="14" t="s">
-        <v>17</v>
-      </c>
+      <c r="AT6" s="14"/>
       <c r="AU6" s="12"/>
-      <c r="AV6" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="AV6" s="11"/>
       <c r="AW6" s="12"/>
       <c r="AX6" s="11"/>
       <c r="AY6" s="12"/>
       <c r="AZ6" s="11"/>
-      <c r="BA6" s="15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BA6" s="15"/>
+    </row>
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="11" t="s">
         <v>18</v>
@@ -1623,22 +1608,16 @@
       <c r="AS7" s="5">
         <v>5</v>
       </c>
-      <c r="AT7" s="10" t="s">
-        <v>18</v>
-      </c>
+      <c r="AT7" s="10"/>
       <c r="AU7" s="11"/>
       <c r="AV7" s="12"/>
       <c r="AW7" s="11"/>
-      <c r="AX7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="AY7" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="AX7" s="12"/>
+      <c r="AY7" s="11"/>
       <c r="AZ7" s="12"/>
       <c r="BA7" s="13"/>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
       <c r="B8" s="12" t="s">
         <v>18</v>
@@ -1702,18 +1681,14 @@
       </c>
       <c r="AT8" s="14"/>
       <c r="AU8" s="12"/>
-      <c r="AV8" s="11" t="s">
-        <v>18</v>
-      </c>
+      <c r="AV8" s="11"/>
       <c r="AW8" s="12"/>
       <c r="AX8" s="11"/>
       <c r="AY8" s="12"/>
-      <c r="AZ8" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="AZ8" s="11"/>
       <c r="BA8" s="15"/>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>16</v>
       </c>
@@ -1782,9 +1757,7 @@
       </c>
       <c r="AU9" s="17"/>
       <c r="AV9" s="18"/>
-      <c r="AW9" s="17" t="s">
-        <v>18</v>
-      </c>
+      <c r="AW9" s="17"/>
       <c r="AX9" s="18"/>
       <c r="AY9" s="17"/>
       <c r="AZ9" s="18"/>
@@ -1792,7 +1765,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="G11" s="27" t="s">
         <v>25</v>
       </c>
@@ -1826,7 +1799,7 @@
       <c r="AI11" s="27"/>
       <c r="AJ11" s="27"/>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="G12" s="27"/>
       <c r="H12" s="27"/>
       <c r="I12" s="27"/>
@@ -1858,7 +1831,7 @@
       <c r="AI12" s="27"/>
       <c r="AJ12" s="27"/>
     </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
       <c r="G13" s="27"/>
       <c r="H13" s="27"/>
       <c r="I13" s="27"/>
@@ -1890,7 +1863,7 @@
       <c r="AI13" s="27"/>
       <c r="AJ13" s="27"/>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="G14" s="27"/>
       <c r="H14" s="27"/>
       <c r="I14" s="27"/>

</xml_diff>

<commit_message>
Add TODO list in Plan B Notes.txt
</commit_message>
<xml_diff>
--- a/Planning/Planning.xlsx
+++ b/Planning/Planning.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584C5119-0880-4482-893D-75C67E646FA8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6194F97-C83D-4328-A2EB-924CAC4D1E83}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -183,7 +183,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,13 +230,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -432,7 +425,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -510,9 +503,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1076,7 +1066,7 @@
   <dimension ref="A1:BA26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AS1" zoomScale="385" zoomScaleNormal="385" workbookViewId="0">
-      <selection activeCell="AW2" sqref="AW2"/>
+      <selection activeCell="AZ5" sqref="AZ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,12 +1427,10 @@
       <c r="AV5" s="12"/>
       <c r="AW5" s="11"/>
       <c r="AX5" s="12"/>
-      <c r="AY5" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="AZ5" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="AY5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="AZ5" s="12"/>
       <c r="BA5" s="13"/>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.25">

</xml_diff>